<commit_message>
Har lavet et udkast til en invitation, samt opdateret budgettet.
</commit_message>
<xml_diff>
--- a/Sommerlejr_budget.xlsx
+++ b/Sommerlejr_budget.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="0" windowWidth="18120" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="3200" yWindow="0" windowWidth="18120" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="Budget" sheetId="1" r:id="rId1"/>
+    <sheet name="Uge Program" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>Enhed</t>
   </si>
@@ -60,6 +61,9 @@
     <t xml:space="preserve">Børn </t>
   </si>
   <si>
+    <t>Ledere</t>
+  </si>
+  <si>
     <t>Antal pers</t>
   </si>
   <si>
@@ -79,6 +83,57 @@
   </si>
   <si>
     <t>MED LEDERE</t>
+  </si>
+  <si>
+    <t>Tid</t>
+  </si>
+  <si>
+    <t>Lørdag</t>
+  </si>
+  <si>
+    <t>Søndag</t>
+  </si>
+  <si>
+    <t>Mandag</t>
+  </si>
+  <si>
+    <t>Tirsdag</t>
+  </si>
+  <si>
+    <t>Onsdag</t>
+  </si>
+  <si>
+    <t>Torsdag</t>
+  </si>
+  <si>
+    <t>Fredag</t>
+  </si>
+  <si>
+    <t>Afgang fra Hou Havn kl 09:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mød din nye gren - aktiviteter med din nye gren </t>
+  </si>
+  <si>
+    <t>Afgang fra Havnen i sælvig kl:13:15</t>
+  </si>
+  <si>
+    <t>Lejr Etablering i grenen</t>
+  </si>
+  <si>
+    <t>Start af tema - Hobbitten</t>
+  </si>
+  <si>
+    <t>Farvel til de små afgang fra Havnen i Sælvig kl:13:15</t>
+  </si>
+  <si>
+    <t>Nedbrydning af lejr for alle</t>
+  </si>
+  <si>
+    <t>Ud i det blå</t>
+  </si>
+  <si>
+    <t>Overnatning på Natur grunden</t>
   </si>
 </sst>
 </file>
@@ -89,8 +144,16 @@
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;kr&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;kr&quot;;[Red]#,##0.00\ &quot;kr&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -113,16 +176,57 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -134,6 +238,21 @@
       <left style="medium">
         <color auto="1"/>
       </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right/>
       <top style="medium">
         <color auto="1"/>
@@ -210,58 +329,182 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Besøgt link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besøgt link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besøgt link" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Besøgt link" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Besøgt link" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Besøgt link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -593,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -607,14 +850,14 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -687,7 +930,9 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5">
         <v>10</v>
@@ -701,7 +946,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5">
@@ -717,7 +962,7 @@
         <v>60</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5">
@@ -927,14 +1172,14 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
       <c r="F14" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -1031,7 +1276,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="7">
@@ -1047,7 +1292,7 @@
         <v>14040</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="7">
@@ -1123,7 +1368,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="7">
@@ -1139,7 +1384,7 @@
         <v>500</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="7">
@@ -1157,7 +1402,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="7">
@@ -1173,7 +1418,7 @@
         <v>234</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="7">
@@ -1284,4 +1529,304 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="39"/>
+    <col min="2" max="9" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="39" customFormat="1" ht="16" thickBot="1">
+      <c r="A1" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="42">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="33"/>
+      <c r="H2" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="33"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="43"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="34"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="43"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="34"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="43"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="34"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="43"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="34"/>
+    </row>
+    <row r="7" spans="1:9" ht="16" thickBot="1">
+      <c r="A7" s="43"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="34"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="43"/>
+      <c r="B8" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="34"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="43"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="34"/>
+    </row>
+    <row r="10" spans="1:9" ht="16" thickBot="1">
+      <c r="A10" s="43"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="34"/>
+    </row>
+    <row r="11" spans="1:9" ht="16" thickBot="1">
+      <c r="A11" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="31"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="35"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="43"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="43"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="16"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="43"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="16"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="43"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="43"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="43"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="16"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="43"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="43"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" spans="1:9" ht="16" thickBot="1">
+      <c r="A20" s="44">
+        <v>0.75</v>
+      </c>
+      <c r="B20" s="23"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="I2:I11"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="I12:I20"/>
+    <mergeCell ref="D2:D20"/>
+    <mergeCell ref="B8:B20"/>
+    <mergeCell ref="C2:C20"/>
+    <mergeCell ref="E2:E10"/>
+    <mergeCell ref="E11:E20"/>
+    <mergeCell ref="F2:F20"/>
+    <mergeCell ref="G2:G20"/>
+    <mergeCell ref="H2:H20"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>